<commit_message>
updates 1, added step 2
</commit_message>
<xml_diff>
--- a/data/20200117-EngiExcel-step0.xlsx
+++ b/data/20200117-EngiExcel-step0.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klee38\excel-engineers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401C4FC7-E27A-430A-B364-B32190E35C2C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212C32F3-0A04-4430-8878-118F40D99CD9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBFE83E4-9E70-4178-B3C6-F36C16CEE212}"/>
+    <workbookView xWindow="31425" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{CBFE83E4-9E70-4178-B3C6-F36C16CEE212}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dist_Widgets" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -93,12 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CD939B-0972-4DBA-B2E6-9D3E267AE425}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,13 +449,13 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>26</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>37</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>64</v>
       </c>
     </row>
@@ -485,6 +486,9 @@
       <c r="E6" s="4">
         <v>53</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>